<commit_message>
Update pie charts to donut charts
</commit_message>
<xml_diff>
--- a/5_Client_Deliverables/Final_report_Instacart_Project.xlsx
+++ b/5_Client_Deliverables/Final_report_Instacart_Project.xlsx
@@ -3874,7 +3874,7 @@
     <xdr:ext cx="3914775" cy="2733675"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image8.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image12.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3930,7 +3930,7 @@
     <xdr:ext cx="4057650" cy="2943225"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image5.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -3978,62 +3978,6 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>276225</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="2790825" cy="1933575"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image9.png" title="Image"/>
-        <xdr:cNvPicPr preferRelativeResize="0"/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId6"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>904875</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>276225</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="2857500" cy="1933575"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image22.png" title="Image"/>
-        <xdr:cNvPicPr preferRelativeResize="0"/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId7"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
       <xdr:row>78</xdr:row>
@@ -4042,11 +3986,11 @@
     <xdr:ext cx="4724400" cy="2809875"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image11.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId8"/>
+        <a:blip cstate="print" r:embed="rId6"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -4070,11 +4014,11 @@
     <xdr:ext cx="4600575" cy="2809875"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image5.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image8.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId9"/>
+        <a:blip cstate="print" r:embed="rId7"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -4098,11 +4042,11 @@
     <xdr:ext cx="4057650" cy="3009900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image25.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image19.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId10"/>
+        <a:blip cstate="print" r:embed="rId8"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -4126,7 +4070,63 @@
     <xdr:ext cx="4057650" cy="3057525"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image23.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image22.png" title="Image"/>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip cstate="print" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2324100" cy="1600200"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="image13.png" title="Image"/>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip cstate="print" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2324100" cy="1600200"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="image18.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4662,157 +4662,17 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>257175</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="3733800" cy="2028825"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image15.png" title="Image"/>
-        <xdr:cNvPicPr preferRelativeResize="0"/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="2362200" cy="2028825"/>
+    <xdr:ext cx="4371975" cy="3209925"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="0" name="image7.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>257175</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="4371975" cy="3209925"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image12.png" title="Image"/>
-        <xdr:cNvPicPr preferRelativeResize="0"/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId5"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>238125</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="2276475" cy="1381125"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image13.png" title="Image"/>
-        <xdr:cNvPicPr preferRelativeResize="0"/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId6"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>828675</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>238125</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="2276475" cy="1381125"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image10.png" title="Image"/>
-        <xdr:cNvPicPr preferRelativeResize="0"/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId7"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>781050</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>238125</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="2276475" cy="1428750"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image17.png" title="Image"/>
-        <xdr:cNvPicPr preferRelativeResize="0"/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId8"/>
+        <a:blip cstate="print" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -4836,11 +4696,11 @@
     <xdr:ext cx="4238625" cy="3438525"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image14.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image15.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId9"/>
+        <a:blip cstate="print" r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -4864,11 +4724,11 @@
     <xdr:ext cx="4238625" cy="3438525"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image16.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image14.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId10"/>
+        <a:blip cstate="print" r:embed="rId5"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -4892,11 +4752,11 @@
     <xdr:ext cx="4238625" cy="1276350"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image24.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image11.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId11"/>
+        <a:blip cstate="print" r:embed="rId6"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -4920,11 +4780,11 @@
     <xdr:ext cx="4086225" cy="3057525"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image21.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image10.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId12"/>
+        <a:blip cstate="print" r:embed="rId7"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -4948,11 +4808,11 @@
     <xdr:ext cx="5695950" cy="1857375"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image18.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image9.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId13"/>
+        <a:blip cstate="print" r:embed="rId8"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -4976,11 +4836,11 @@
     <xdr:ext cx="4705350" cy="2114550"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image20.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image16.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId14"/>
+        <a:blip cstate="print" r:embed="rId9"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -5004,7 +4864,147 @@
     <xdr:ext cx="4057650" cy="3057525"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image19.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image17.png" title="Image"/>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip cstate="print" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3629025" cy="1990725"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="image23.png" title="Image"/>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip cstate="print" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2133600" cy="1990725"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="image20.png" title="Image"/>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip cstate="print" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2381250" cy="1457325"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="image21.png" title="Image"/>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip cstate="print" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2381250" cy="1457325"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="image24.png" title="Image"/>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip cstate="print" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2533650" cy="1457325"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="image25.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>

</xml_diff>